<commit_message>
The final version of web scraping assignment
</commit_message>
<xml_diff>
--- a/assignments/Assignment 3 Data Visualization + Web-scraping/bama-cars-samand.xlsx
+++ b/assignments/Assignment 3 Data Visualization + Web-scraping/bama-cars-samand.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Teias\Usage\Term-1\ADS\Assignments\ads-course\assignments\Assignment 3 Data Visualization + Web-scraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4EA82E4-5A7A-4EAF-8495-0101DD77FB24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E79C1E-E1D9-4089-94C7-4D307D9A8F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="78">
   <si>
     <t>Title</t>
   </si>
@@ -70,30 +70,72 @@
     <t>داخل کرم</t>
   </si>
   <si>
+    <t>نقره ای</t>
+  </si>
+  <si>
+    <t>چند لکه رنگ</t>
+  </si>
+  <si>
+    <t>سمند، سورن</t>
+  </si>
+  <si>
+    <t>داخل مشکی</t>
+  </si>
+  <si>
+    <t>فول شرکتی رینگ آلومینیومی مانیتور فابریک و دوربین دنده عقب کروز کنترل  صندلی برقی</t>
+  </si>
+  <si>
+    <t>دوگانه سوز</t>
+  </si>
+  <si>
+    <t>یک لکه رنگ</t>
+  </si>
+  <si>
+    <t>از سال 94دست خودم بوذه تازه موتور و جلوبندی و دیسک و تسمه تایم و لوازم مصرفی عوض شده. درب راننده رو بخاطر فرورفتگی عوض کردم. خط و خش هم دارد. قیمت هم با خریدار راه میام با تیبا و ساینا و کوییک صفر هم معاوضه دارم بازدید هم اسلام اباد غرب</t>
+  </si>
+  <si>
+    <t>با رینگ،یکسال بیمه</t>
+  </si>
+  <si>
+    <t>داخل خاکستری</t>
+  </si>
+  <si>
+    <t>روکش صندلی  دودی هدلایت منبع اگزوز HKS همه روشه ماشین از پشت ضربه خورده با مشتری واقعی کنار میایم با تشکر</t>
+  </si>
+  <si>
+    <t>داخل قهوه ای</t>
+  </si>
+  <si>
+    <t>ماشین فوق‌العاده سالم تماس سرویس ها به موقع  انجام شده</t>
+  </si>
+  <si>
+    <t>داخل نوک مدادی</t>
+  </si>
+  <si>
+    <t>ماشین صحیح وسالم ، فوری فروشی ، زیر قیمت .</t>
+  </si>
+  <si>
+    <t>خاکستری</t>
+  </si>
+  <si>
+    <t>از صفر دست خودم بوده رینگ آلومینیومی صلیبی بدون تصادف دو درب بدون رنگ صافکاری جزئی دارد کفپوش 3D داخل کابین و صندوق</t>
+  </si>
+  <si>
+    <t>گلگیر رنگ</t>
+  </si>
+  <si>
+    <t>ماشین جلوگلگیرهارنگ.سینی پشت چراغ رنگ سمت شاگرد یه ضربه جزئی داشته.شاسی نه جوش خورده ن اصلا شکسته ن ترک داره توبرگه کارشناسی خورده فقط ی زربه جزئی سرشاسی مابقی ب شرط سالم.ماشین بقیه جاهاکاملا.بیرنگ وضربه.سند تک برگ ب نسبت مدل کم کار.دوستان توجه کنید ماشین۱هفته است ازنمایندگیef7آوردم بافاکتور.۶۰ملیون هزینه کردم که تو سرماشین نزنن تاکوچکترین قطعات تعویض شده جانمیشه بنویسم.تمام ادوات برقی درحدنو.ماشین رینگ و سیستم روش هست.کولر وبخاری هیولا.دوگانه شرکت.ماشین درحد صفر به شرط هر کارشناسی ک بخواین.</t>
+  </si>
+  <si>
     <t>بدون خرج،با دنا پلاس تیپ یک هم معاوضه میکنم</t>
   </si>
   <si>
-    <t>داخل قهوه ای</t>
-  </si>
-  <si>
     <t>سند تک برگ. دیسک صفحه والوو 2 ماه تعویض-تسمه تایم تعویض- باطری 3 ماه تعویض مارک سوزوکی 72 امپر- شیشه ها دودی 40% لاستیک 205 کویر 70% - بیمه تا برج 2 سال 1403 و معاینه فنی تا برج 3 سال 1403- کفپایی سه بعدی- از لحاظ موتوری سالم و به شرط - مصرفی خودم بوده</t>
   </si>
   <si>
-    <t>سمند، سورن</t>
-  </si>
-  <si>
-    <t>دوگانه سوز</t>
-  </si>
-  <si>
-    <t>داخل مشکی</t>
-  </si>
-  <si>
     <t>◻︎◻︎ خشک … پلاکـ شده ☐☐فروش نقدی و تحویل همان لحظه یک ساعته ☐(سند ازاد) با گارانتی و بیمه شخص ثالث ✔️✔️☐☐ . 1️⃣روییت خودرو ..2️⃣تحویل خودرو … 3️⃣تسویه مبلغ … ✔️ساعت کاری ٩صبح الی ٧ عصر ☐☐.. ⚬دوستان لطفا توجه کنید ، با دلال و کاسب هیچ همکاری نمیشود⚬⚬ خودرو فقط به شخص مصرف کننده فروخته میشود⚬</t>
   </si>
   <si>
-    <t>یک لکه رنگ</t>
-  </si>
-  <si>
     <t>دارای مانیتور</t>
   </si>
   <si>
@@ -127,9 +169,6 @@
     <t>مشکی</t>
   </si>
   <si>
-    <t>خاکستری</t>
-  </si>
-  <si>
     <t>سند دست اول ،شاسی پلمپ ،تمام سرویس ها به موقع ،کم کارکرد ،سرویس کامل جلوبندی ،فقط مصرف کننده ،تخفیف پای معامله</t>
   </si>
   <si>
@@ -157,9 +196,6 @@
     <t>صافکاری بدون رنگ</t>
   </si>
   <si>
-    <t>داخل خاکستری</t>
-  </si>
-  <si>
     <t>ماشین کاملا خانوادگی از صفر دست خودم بوده برای مسافرت.کم کار و سالم.سرویس ها به موقع انجام شده.لاستیک حدود 80 درصد بیمه تا برج 11.درب سمت شاگرد قسمت پایین به اندازه یک کف دست صافکاری بدون رنگ داشته.خط و خش جزئی</t>
   </si>
   <si>
@@ -175,30 +211,9 @@
     <t>تحویل فوری ۱ ساعته۵۰ درصد نقد مابقی اقساط ۴ تا ۱۴ ماه مدارک به نام خریدار فقط چک بدون ضامن پرداخت اقساط هر ۳ماه یکبار تهران و شهرستان در صورت نداشتن چک می توانید از چک شخص دیگری استفاده کنید.با امکان تسویه زودتر از موعد با کسر سودبه دلیل نوسان شدید ، قیمت ها حدودی می باشدساعت تماس همه روزه از ۹ صبح تا ۲۰</t>
   </si>
   <si>
-    <t>گلگیر رنگ</t>
-  </si>
-  <si>
-    <t>ماشین جلوگلگیرهارنگ.سینی پشت چراغ رنگ سمت شاگرد یه ضربه جزئی داشته.شاسی نه جوش خورده ن اصلا شکسته ن ترک داره توبرگه کارشناسی خورده فقط ی زربه جزئی سرشاسی مابقی ب شرط سالم.ماشین بقیه جاهاکاملا.بیرنگ وضربه.سند تک برگ ب نسبت مدل کم کار.دوستان توجه کنید ماشین۱هفته است ازنمایندگیef7آوردم بافاکتور.۶۰ملیون هزینه کردم که تو سرماشین نزنن تاکوچکترین قطعات تعویض شده جانمیشه بنویسم.تمام ادوات برقی درحدنو.ماشین رینگ و سیستم روش هست.کولر وبخاری هیولا.دوگانه شرکت.ماشین درحد صفر به شرط هر کارشناسی ک بخواین.</t>
-  </si>
-  <si>
     <t>کم کارکرد-مولتی پلکس برگه کارشناسی بدنه سالم و بدون هیچگونه ضربه.فنی سالم و تعویضی ها انجام شده سالم و خونگی</t>
   </si>
   <si>
-    <t>از صفر دست خودم بوده رینگ آلومینیومی صلیبی بدون تصادف دو درب بدون رنگ صافکاری جزئی دارد کفپوش 3D داخل کابین و صندوق</t>
-  </si>
-  <si>
-    <t>روکش صندلی  دودی هدلایت منبع اگزوز HKS همه روشه ماشین از پشت ضربه خورده با مشتری واقعی کنار میایم با تشکر</t>
-  </si>
-  <si>
-    <t>ماشین صحیح وسالم ، فوری فروشی ، زیر قیمت .</t>
-  </si>
-  <si>
-    <t>داخل نوک مدادی</t>
-  </si>
-  <si>
-    <t>ماشین فوق‌العاده سالم تماس سرویس ها به موقع  انجام شده</t>
-  </si>
-  <si>
     <t>در حد صفر</t>
   </si>
   <si>
@@ -208,9 +223,6 @@
     <t>با مدل بالا دوگانه معاویضه میکنم</t>
   </si>
   <si>
-    <t>چند لکه رنگ</t>
-  </si>
-  <si>
     <t>سنداول ۷سال تخفیف بیمه معاینه برتر۶ماه بیمه ۳ماه لاستیکها ۴۰درصد خط وخش جزیی دارای لوازم اضافه شامل یک حلقه لاستیک کویر۶۰درصد کمپرسوربادفندکی جاروفندکی کابل باتری به باتری سیم بکسل وچراغ دوره گردویک مجموعه کامل لوازم جلوبندی میشلن سند قطعی بنام خریدار فقط جهت مصرف کننده واقعی از پاسخگویی به دلال ونمایشگاهی معذورم</t>
   </si>
   <si>
@@ -242,21 +254,6 @@
   </si>
   <si>
     <t>لوازم بوش آلمان خودرو کاملا سالم و بدون خرج، کابین بدون سرصدا  سه لکه رنگ،کاپوت و دو گلگیر جلو(ترافیکی)بدون ضربه لاستیک ها ۸۰٪  زیرپایی سه بعدی،روکش صندلی شاسی ها به شرط کارشناسی تمام مصرفی ها تعویض شده آفتاب سوختگی در سقف و قسمتی از صندوق تخفیف پای معامله توضیحات کامله،خریدار واقعی،مصرف کننده تماس بگیره جهت بازدید ۵ عصر به بعد در خدمتم</t>
-  </si>
-  <si>
-    <t>کلیه قطعات فعال ! بیمه و معاینه برج3 لاستیک 205 دزدگیر پاور ویندوز یک لکه رنگ به اندازه کف دست روی گلگیر+قلم کاری جزئی روی کاپوت خط و خش و مالیدگی جزئی دارد! شاسی ها پلمپ بدون ضربه کابین بدون کوچکترین صدا خودرو به شرط مکانیک وکارشناس.</t>
-  </si>
-  <si>
-    <t>کروز کنترل- 2 ایربگ - سنسور عقب -توزیع نیرو ترمز- آینه جانبی تاشو برقی- آینه جانبی با گرمکن -آینه جانبی با تنظیم برقی- ترمز ضدقفل - ایزوفیکس صندلی- دی لایت - چراغ مه‌شکن جلو و عقب – سیستم صوتی پخش جدید با خروجی ساب ووفر- قابلیت پشتیبانی (- (Bluetooth - CD - MP3مدارک کامل و آماده انتقال سند. فروش نقد.اقساط-و برای بازدید از سایر خودروها با شماره مجموعه تماس حاصل فرمایید. بازدید همه روزه از ساعت 8:30 الی 20</t>
-  </si>
-  <si>
-    <t>بیمه تا 29 بهمن معاینه فنی تا 10اسفند تمام مصرفی ها تعویض شده 1_تسمه تایم2_تسمه دینام3_هرزگرد۴_دیسک صفحه بهترین جنس اصلی 5_جلوبندی کامل سرویس شده6_رادیاتور هردوتعویض شده هم موتور وهم رادیاتور بخاری7_شمع ها سوزنی و ایر شمع نو شده8_موتور تقویت شده فوق العاده پرشتاب9_رینگ اسپرت لاستیک 205هست10_سیم کلاچ گیربکسی شده فوق العاده نرم درب عقب سمت شاگرد از دستگیره رنگ</t>
-  </si>
-  <si>
-    <t>به صورت نقد.اقساط تهران وشهرستان/حداقل پیش پرداخت 30%قیمت روزخودرو/بیمه شخص ثالث+70%تخفیف بیمه بدنه/امکان تسویه زودترازموعدباکسرسود/کلیه خودروهاشامل گارانتی وخدمات پس ازفروش میباشند/ارسال خودرو باخودروبرتادرب منزل درصورت تمایل خریداردرتهران وحومه رایگان میباشد/باتوجه به نوسانات قیمت بازار برای استعلام قیمت تماس حاصل فرمایید.</t>
-  </si>
-  <si>
-    <t>ماشین شخصی هست لطفا فقط تماس بگیرید</t>
   </si>
 </sst>
 </file>
@@ -621,14 +618,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="9" max="9" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -671,7 +673,7 @@
         <v>10</v>
       </c>
       <c r="C2">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -688,11 +690,8 @@
       <c r="H2" t="s">
         <v>15</v>
       </c>
-      <c r="I2">
-        <v>78000</v>
-      </c>
       <c r="K2">
-        <v>410000000</v>
+        <v>383000000</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -703,7 +702,7 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>1396</v>
+        <v>1390</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -712,19 +711,19 @@
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H3" t="s">
         <v>15</v>
       </c>
-      <c r="J3" t="s">
-        <v>16</v>
+      <c r="I3">
+        <v>400000</v>
       </c>
       <c r="K3">
-        <v>380000000</v>
+        <v>230000000</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -732,10 +731,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C4">
-        <v>1395</v>
+        <v>1402</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -750,16 +749,13 @@
         <v>14</v>
       </c>
       <c r="H4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4">
-        <v>203000</v>
+        <v>19</v>
       </c>
       <c r="J4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K4">
-        <v>310000000</v>
+        <v>579000000</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -767,13 +763,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C5">
-        <v>1402</v>
+        <v>1394</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
@@ -782,16 +778,19 @@
         <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H5" t="s">
-        <v>21</v>
+        <v>15</v>
+      </c>
+      <c r="I5">
+        <v>217000</v>
       </c>
       <c r="J5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K5">
-        <v>575000000</v>
+        <v>325000000</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -799,10 +798,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C6">
-        <v>1397</v>
+        <v>1401</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -814,13 +813,16 @@
         <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="H6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6">
-        <v>106000</v>
+        <v>19</v>
+      </c>
+      <c r="J6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6">
+        <v>550000000</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -828,10 +830,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7">
-        <v>1402</v>
+        <v>1395</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
@@ -843,16 +845,16 @@
         <v>13</v>
       </c>
       <c r="G7" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H7" t="s">
-        <v>21</v>
+        <v>25</v>
+      </c>
+      <c r="I7">
+        <v>160000</v>
       </c>
       <c r="J7" t="s">
-        <v>24</v>
-      </c>
-      <c r="K7">
-        <v>584000000</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -860,10 +862,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C8">
-        <v>1394</v>
+        <v>1397</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
@@ -872,19 +874,22 @@
         <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="G8" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="H8" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="I8">
-        <v>100000</v>
+        <v>240000</v>
       </c>
       <c r="J8" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="K8">
+        <v>380000000</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -895,10 +900,10 @@
         <v>10</v>
       </c>
       <c r="C9">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E9" t="s">
         <v>12</v>
@@ -910,16 +915,13 @@
         <v>14</v>
       </c>
       <c r="H9" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="I9">
-        <v>70000</v>
-      </c>
-      <c r="J9" t="s">
-        <v>28</v>
+        <v>112000</v>
       </c>
       <c r="K9">
-        <v>445000000</v>
+        <v>395000000</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -930,7 +932,7 @@
         <v>10</v>
       </c>
       <c r="C10">
-        <v>1390</v>
+        <v>1400</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
@@ -939,22 +941,22 @@
         <v>12</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="G10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10">
+        <v>46000</v>
+      </c>
+      <c r="J10" t="s">
         <v>30</v>
       </c>
-      <c r="H10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10">
-        <v>203000</v>
-      </c>
-      <c r="J10" t="s">
-        <v>31</v>
-      </c>
       <c r="K10">
-        <v>270000000</v>
+        <v>385000000</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -965,7 +967,7 @@
         <v>10</v>
       </c>
       <c r="C11">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="D11" t="s">
         <v>11</v>
@@ -974,19 +976,19 @@
         <v>12</v>
       </c>
       <c r="F11" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="G11" t="s">
         <v>14</v>
       </c>
       <c r="H11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11">
+        <v>180000</v>
+      </c>
+      <c r="J11" t="s">
         <v>32</v>
-      </c>
-      <c r="I11">
-        <v>112313</v>
-      </c>
-      <c r="J11" t="s">
-        <v>33</v>
       </c>
       <c r="K11">
         <v>390000000</v>
@@ -1000,28 +1002,28 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>1399</v>
+        <v>1388</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E12" t="s">
         <v>12</v>
       </c>
       <c r="F12" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="G12" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H12" t="s">
         <v>15</v>
       </c>
       <c r="I12">
-        <v>130000</v>
+        <v>390000</v>
       </c>
       <c r="K12">
-        <v>390000000</v>
+        <v>215000000</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1032,31 +1034,31 @@
         <v>10</v>
       </c>
       <c r="C13">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>
       </c>
       <c r="F13" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="G13" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="H13" t="s">
         <v>15</v>
       </c>
       <c r="I13">
-        <v>90000</v>
+        <v>222000</v>
       </c>
       <c r="J13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K13">
-        <v>390000000</v>
+        <v>350000000</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1067,10 +1069,10 @@
         <v>10</v>
       </c>
       <c r="C14">
-        <v>1389</v>
+        <v>1399</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E14" t="s">
         <v>12</v>
@@ -1079,16 +1081,16 @@
         <v>13</v>
       </c>
       <c r="G14" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="H14" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="I14">
-        <v>230000</v>
-      </c>
-      <c r="J14" t="s">
-        <v>39</v>
+        <v>78000</v>
+      </c>
+      <c r="K14">
+        <v>410000000</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -1096,10 +1098,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C15">
-        <v>1401</v>
+        <v>1396</v>
       </c>
       <c r="D15" t="s">
         <v>11</v>
@@ -1114,13 +1116,16 @@
         <v>14</v>
       </c>
       <c r="H15" t="s">
-        <v>21</v>
+        <v>15</v>
+      </c>
+      <c r="I15">
+        <v>210000</v>
       </c>
       <c r="J15" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="K15">
-        <v>550000000</v>
+        <v>380000000</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -1128,34 +1133,28 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>1397</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" t="s">
         <v>19</v>
       </c>
-      <c r="C16">
-        <v>1400</v>
-      </c>
-      <c r="D16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" t="s">
-        <v>14</v>
-      </c>
-      <c r="H16" t="s">
-        <v>21</v>
-      </c>
       <c r="I16">
-        <v>52000</v>
-      </c>
-      <c r="J16" t="s">
-        <v>41</v>
-      </c>
-      <c r="K16">
-        <v>480000000</v>
+        <v>106000</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -1166,10 +1165,10 @@
         <v>10</v>
       </c>
       <c r="C17">
-        <v>1390</v>
+        <v>1395</v>
       </c>
       <c r="D17" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E17" t="s">
         <v>12</v>
@@ -1178,16 +1177,19 @@
         <v>13</v>
       </c>
       <c r="G17" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="H17" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="I17">
-        <v>395000</v>
+        <v>203000</v>
       </c>
       <c r="J17" t="s">
-        <v>43</v>
+        <v>36</v>
+      </c>
+      <c r="K17">
+        <v>310000000</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -1195,13 +1197,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C18">
-        <v>1393</v>
+        <v>1402</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E18" t="s">
         <v>12</v>
@@ -1210,19 +1212,16 @@
         <v>13</v>
       </c>
       <c r="G18" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="H18" t="s">
-        <v>45</v>
-      </c>
-      <c r="I18">
-        <v>145000</v>
+        <v>19</v>
       </c>
       <c r="J18" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="K18">
-        <v>300000000</v>
+        <v>575000000</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -1230,10 +1229,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C19">
-        <v>1393</v>
+        <v>1402</v>
       </c>
       <c r="D19" t="s">
         <v>11</v>
@@ -1248,13 +1247,13 @@
         <v>14</v>
       </c>
       <c r="H19" t="s">
-        <v>15</v>
-      </c>
-      <c r="I19">
-        <v>190000</v>
+        <v>19</v>
       </c>
       <c r="J19" t="s">
-        <v>47</v>
+        <v>38</v>
+      </c>
+      <c r="K19">
+        <v>584000000</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -1262,10 +1261,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C20">
-        <v>1389</v>
+        <v>1394</v>
       </c>
       <c r="D20" t="s">
         <v>11</v>
@@ -1274,22 +1273,19 @@
         <v>12</v>
       </c>
       <c r="F20" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="G20" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H20" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="I20">
-        <v>225000</v>
+        <v>100000</v>
       </c>
       <c r="J20" t="s">
-        <v>48</v>
-      </c>
-      <c r="K20">
-        <v>250000000</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -1300,10 +1296,10 @@
         <v>10</v>
       </c>
       <c r="C21">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="D21" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E21" t="s">
         <v>12</v>
@@ -1318,10 +1314,13 @@
         <v>15</v>
       </c>
       <c r="I21">
-        <v>80000</v>
+        <v>70000</v>
       </c>
       <c r="J21" t="s">
-        <v>49</v>
+        <v>42</v>
+      </c>
+      <c r="K21">
+        <v>445000000</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -1329,10 +1328,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C22">
-        <v>1402</v>
+        <v>1390</v>
       </c>
       <c r="D22" t="s">
         <v>11</v>
@@ -1341,19 +1340,22 @@
         <v>12</v>
       </c>
       <c r="F22" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="G22" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="H22" t="s">
-        <v>21</v>
+        <v>15</v>
+      </c>
+      <c r="I22">
+        <v>203000</v>
       </c>
       <c r="J22" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="K22">
-        <v>285000000</v>
+        <v>270000000</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -1364,10 +1366,10 @@
         <v>10</v>
       </c>
       <c r="C23">
-        <v>1395</v>
+        <v>1398</v>
       </c>
       <c r="D23" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E23" t="s">
         <v>12</v>
@@ -1376,19 +1378,19 @@
         <v>13</v>
       </c>
       <c r="G23" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="H23" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="I23">
-        <v>222000</v>
+        <v>112313</v>
       </c>
       <c r="J23" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="K23">
-        <v>200000000</v>
+        <v>390000000</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -1399,16 +1401,16 @@
         <v>10</v>
       </c>
       <c r="C24">
-        <v>1394</v>
+        <v>1399</v>
       </c>
       <c r="D24" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E24" t="s">
         <v>12</v>
       </c>
       <c r="F24" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="G24" t="s">
         <v>14</v>
@@ -1417,13 +1419,10 @@
         <v>15</v>
       </c>
       <c r="I24">
-        <v>90000</v>
-      </c>
-      <c r="J24" t="s">
-        <v>53</v>
+        <v>130000</v>
       </c>
       <c r="K24">
-        <v>320000000</v>
+        <v>390000000</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -1434,31 +1433,31 @@
         <v>10</v>
       </c>
       <c r="C25">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="D25" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E25" t="s">
         <v>12</v>
       </c>
       <c r="F25" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G25" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H25" t="s">
         <v>15</v>
       </c>
       <c r="I25">
-        <v>180000</v>
+        <v>91000</v>
       </c>
       <c r="J25" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="K25">
-        <v>390000000</v>
+        <v>385000000</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
@@ -1466,13 +1465,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C26">
-        <v>1395</v>
+        <v>1389</v>
       </c>
       <c r="D26" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E26" t="s">
         <v>12</v>
@@ -1481,16 +1480,16 @@
         <v>13</v>
       </c>
       <c r="G26" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="H26" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="I26">
-        <v>160000</v>
+        <v>230000</v>
       </c>
       <c r="J26" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -1498,10 +1497,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C27">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -1516,16 +1515,13 @@
         <v>14</v>
       </c>
       <c r="H27" t="s">
-        <v>15</v>
-      </c>
-      <c r="I27">
-        <v>46000</v>
+        <v>19</v>
       </c>
       <c r="J27" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K27">
-        <v>385000000</v>
+        <v>550000000</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -1533,10 +1529,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C28">
-        <v>1397</v>
+        <v>1400</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
@@ -1551,13 +1547,16 @@
         <v>14</v>
       </c>
       <c r="H28" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="I28">
-        <v>112000</v>
+        <v>52000</v>
+      </c>
+      <c r="J28" t="s">
+        <v>54</v>
       </c>
       <c r="K28">
-        <v>395000000</v>
+        <v>480000000</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -1568,10 +1567,10 @@
         <v>10</v>
       </c>
       <c r="C29">
-        <v>1397</v>
+        <v>1390</v>
       </c>
       <c r="D29" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E29" t="s">
         <v>12</v>
@@ -1580,19 +1579,16 @@
         <v>13</v>
       </c>
       <c r="G29" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="H29" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="I29">
-        <v>240000</v>
+        <v>395000</v>
       </c>
       <c r="J29" t="s">
-        <v>58</v>
-      </c>
-      <c r="K29">
-        <v>380000000</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
@@ -1603,7 +1599,7 @@
         <v>10</v>
       </c>
       <c r="C30">
-        <v>1397</v>
+        <v>1393</v>
       </c>
       <c r="D30" t="s">
         <v>11</v>
@@ -1615,13 +1611,19 @@
         <v>13</v>
       </c>
       <c r="G30" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="H30" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="I30">
-        <v>180000</v>
+        <v>145000</v>
+      </c>
+      <c r="J30" t="s">
+        <v>58</v>
+      </c>
+      <c r="K30">
+        <v>300000000</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -1632,7 +1634,7 @@
         <v>10</v>
       </c>
       <c r="C31">
-        <v>1397</v>
+        <v>1393</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
@@ -1647,10 +1649,10 @@
         <v>14</v>
       </c>
       <c r="H31" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="I31">
-        <v>1800</v>
+        <v>190000</v>
       </c>
       <c r="J31" t="s">
         <v>59</v>
@@ -1661,31 +1663,34 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32">
+        <v>1389</v>
+      </c>
+      <c r="D32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" t="s">
+        <v>57</v>
+      </c>
+      <c r="H32" t="s">
+        <v>15</v>
+      </c>
+      <c r="I32">
+        <v>225000</v>
+      </c>
+      <c r="J32" t="s">
         <v>60</v>
       </c>
-      <c r="C32">
-        <v>1393</v>
-      </c>
-      <c r="D32" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32" t="s">
-        <v>13</v>
-      </c>
-      <c r="G32" t="s">
-        <v>14</v>
-      </c>
-      <c r="H32" t="s">
-        <v>15</v>
-      </c>
-      <c r="I32">
-        <v>190000</v>
-      </c>
-      <c r="J32" t="s">
-        <v>61</v>
+      <c r="K32">
+        <v>250000000</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
@@ -1696,7 +1701,7 @@
         <v>10</v>
       </c>
       <c r="C33">
-        <v>1388</v>
+        <v>1399</v>
       </c>
       <c r="D33" t="s">
         <v>11</v>
@@ -1708,16 +1713,16 @@
         <v>13</v>
       </c>
       <c r="G33" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="H33" t="s">
         <v>15</v>
       </c>
       <c r="I33">
-        <v>390000</v>
-      </c>
-      <c r="K33">
-        <v>215000000</v>
+        <v>80000</v>
+      </c>
+      <c r="J33" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
@@ -1725,10 +1730,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C34">
-        <v>1394</v>
+        <v>1402</v>
       </c>
       <c r="D34" t="s">
         <v>11</v>
@@ -1737,19 +1742,19 @@
         <v>12</v>
       </c>
       <c r="F34" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="G34" t="s">
         <v>14</v>
       </c>
       <c r="H34" t="s">
-        <v>38</v>
-      </c>
-      <c r="I34">
-        <v>218000</v>
+        <v>19</v>
+      </c>
+      <c r="J34" t="s">
+        <v>62</v>
       </c>
       <c r="K34">
-        <v>300000000</v>
+        <v>285000000</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
@@ -1760,7 +1765,7 @@
         <v>10</v>
       </c>
       <c r="C35">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="D35" t="s">
         <v>11</v>
@@ -1769,7 +1774,7 @@
         <v>12</v>
       </c>
       <c r="F35" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="G35" t="s">
         <v>14</v>
@@ -1778,13 +1783,13 @@
         <v>15</v>
       </c>
       <c r="I35">
-        <v>160000</v>
+        <v>90000</v>
       </c>
       <c r="J35" t="s">
         <v>63</v>
       </c>
       <c r="K35">
-        <v>340000000</v>
+        <v>320000000</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
@@ -1795,7 +1800,7 @@
         <v>10</v>
       </c>
       <c r="C36">
-        <v>1400</v>
+        <v>1397</v>
       </c>
       <c r="D36" t="s">
         <v>11</v>
@@ -1804,22 +1809,16 @@
         <v>12</v>
       </c>
       <c r="F36" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="G36" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="H36" t="s">
         <v>15</v>
       </c>
       <c r="I36">
-        <v>42000</v>
-      </c>
-      <c r="J36" t="s">
-        <v>64</v>
-      </c>
-      <c r="K36">
-        <v>392000000</v>
+        <v>180000</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
@@ -1827,10 +1826,10 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C37">
-        <v>1401</v>
+        <v>1397</v>
       </c>
       <c r="D37" t="s">
         <v>11</v>
@@ -1845,16 +1844,13 @@
         <v>14</v>
       </c>
       <c r="H37" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="I37">
-        <v>16500</v>
+        <v>1800</v>
       </c>
       <c r="J37" t="s">
-        <v>65</v>
-      </c>
-      <c r="K37">
-        <v>520000000</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
@@ -1862,13 +1858,13 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="C38">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="D38" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E38" t="s">
         <v>12</v>
@@ -1877,19 +1873,16 @@
         <v>13</v>
       </c>
       <c r="G38" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="H38" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I38">
-        <v>215000</v>
+        <v>190000</v>
       </c>
       <c r="J38" t="s">
         <v>66</v>
-      </c>
-      <c r="K38">
-        <v>280000000</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
@@ -1900,28 +1893,28 @@
         <v>10</v>
       </c>
       <c r="C39">
-        <v>1399</v>
+        <v>1394</v>
       </c>
       <c r="D39" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E39" t="s">
         <v>12</v>
       </c>
       <c r="F39" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="G39" t="s">
         <v>14</v>
       </c>
       <c r="H39" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="I39">
-        <v>58000</v>
-      </c>
-      <c r="J39" t="s">
-        <v>67</v>
+        <v>218000</v>
+      </c>
+      <c r="K39">
+        <v>300000000</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
@@ -1932,7 +1925,7 @@
         <v>10</v>
       </c>
       <c r="C40">
-        <v>1398</v>
+        <v>1395</v>
       </c>
       <c r="D40" t="s">
         <v>11</v>
@@ -1941,22 +1934,22 @@
         <v>12</v>
       </c>
       <c r="F40" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="G40" t="s">
         <v>14</v>
       </c>
       <c r="H40" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I40">
-        <v>50000</v>
+        <v>160000</v>
       </c>
       <c r="J40" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K40">
-        <v>370000000</v>
+        <v>330000000</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
@@ -1967,7 +1960,7 @@
         <v>10</v>
       </c>
       <c r="C41">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="D41" t="s">
         <v>11</v>
@@ -1976,19 +1969,22 @@
         <v>12</v>
       </c>
       <c r="F41" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="G41" t="s">
         <v>14</v>
       </c>
       <c r="H41" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I41">
-        <v>49500</v>
+        <v>42000</v>
+      </c>
+      <c r="J41" t="s">
+        <v>68</v>
       </c>
       <c r="K41">
-        <v>385000000</v>
+        <v>392000000</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
@@ -1996,10 +1992,10 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C42">
-        <v>1395</v>
+        <v>1401</v>
       </c>
       <c r="D42" t="s">
         <v>11</v>
@@ -2014,13 +2010,16 @@
         <v>14</v>
       </c>
       <c r="H42" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="I42">
-        <v>130000</v>
+        <v>16500</v>
       </c>
       <c r="J42" t="s">
         <v>69</v>
+      </c>
+      <c r="K42">
+        <v>520000000</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
@@ -2031,10 +2030,10 @@
         <v>10</v>
       </c>
       <c r="C43">
-        <v>1397</v>
+        <v>1394</v>
       </c>
       <c r="D43" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E43" t="s">
         <v>12</v>
@@ -2043,16 +2042,19 @@
         <v>13</v>
       </c>
       <c r="G43" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H43" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="I43">
-        <v>130000</v>
+        <v>215000</v>
+      </c>
+      <c r="J43" t="s">
+        <v>70</v>
       </c>
       <c r="K43">
-        <v>420000000</v>
+        <v>280000000</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
@@ -2063,10 +2065,10 @@
         <v>10</v>
       </c>
       <c r="C44">
-        <v>1394</v>
+        <v>1399</v>
       </c>
       <c r="D44" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E44" t="s">
         <v>12</v>
@@ -2081,13 +2083,10 @@
         <v>15</v>
       </c>
       <c r="I44">
-        <v>173000</v>
+        <v>58000</v>
       </c>
       <c r="J44" t="s">
-        <v>70</v>
-      </c>
-      <c r="K44">
-        <v>300000000</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
@@ -2095,10 +2094,10 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C45">
-        <v>1402</v>
+        <v>1398</v>
       </c>
       <c r="D45" t="s">
         <v>11</v>
@@ -2113,10 +2112,16 @@
         <v>14</v>
       </c>
       <c r="H45" t="s">
-        <v>21</v>
+        <v>27</v>
+      </c>
+      <c r="I45">
+        <v>50000</v>
       </c>
       <c r="J45" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="K45">
+        <v>370000000</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
@@ -2127,28 +2132,28 @@
         <v>10</v>
       </c>
       <c r="C46">
-        <v>1390</v>
+        <v>1399</v>
       </c>
       <c r="D46" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E46" t="s">
         <v>12</v>
       </c>
       <c r="F46" t="s">
-        <v>72</v>
+        <v>13</v>
       </c>
       <c r="G46" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="H46" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="I46">
-        <v>200000</v>
-      </c>
-      <c r="J46" t="s">
-        <v>73</v>
+        <v>49500</v>
+      </c>
+      <c r="K46">
+        <v>385000000</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
@@ -2159,7 +2164,7 @@
         <v>10</v>
       </c>
       <c r="C47">
-        <v>1388</v>
+        <v>1395</v>
       </c>
       <c r="D47" t="s">
         <v>11</v>
@@ -2171,19 +2176,16 @@
         <v>13</v>
       </c>
       <c r="G47" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="H47" t="s">
         <v>15</v>
       </c>
       <c r="I47">
-        <v>186000</v>
+        <v>130000</v>
       </c>
       <c r="J47" t="s">
-        <v>74</v>
-      </c>
-      <c r="K47">
-        <v>230000000</v>
+        <v>73</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
@@ -2191,28 +2193,31 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C48">
-        <v>1402</v>
+        <v>1397</v>
       </c>
       <c r="D48" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E48" t="s">
         <v>12</v>
       </c>
       <c r="F48" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="G48" t="s">
         <v>14</v>
       </c>
       <c r="H48" t="s">
-        <v>21</v>
-      </c>
-      <c r="J48" t="s">
-        <v>75</v>
+        <v>27</v>
+      </c>
+      <c r="I48">
+        <v>130000</v>
+      </c>
+      <c r="K48">
+        <v>420000000</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
@@ -2223,7 +2228,7 @@
         <v>10</v>
       </c>
       <c r="C49">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="D49" t="s">
         <v>11</v>
@@ -2235,19 +2240,19 @@
         <v>13</v>
       </c>
       <c r="G49" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="H49" t="s">
         <v>15</v>
       </c>
       <c r="I49">
-        <v>200000</v>
+        <v>173000</v>
       </c>
       <c r="J49" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K49">
-        <v>330000000</v>
+        <v>300000000</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
@@ -2255,7 +2260,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C50">
         <v>1402</v>
@@ -2273,13 +2278,10 @@
         <v>14</v>
       </c>
       <c r="H50" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J50" t="s">
-        <v>77</v>
-      </c>
-      <c r="K50">
-        <v>168000000</v>
+        <v>75</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
@@ -2290,31 +2292,28 @@
         <v>10</v>
       </c>
       <c r="C51">
-        <v>1394</v>
+        <v>1390</v>
       </c>
       <c r="D51" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E51" t="s">
         <v>12</v>
       </c>
       <c r="F51" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="G51" t="s">
-        <v>62</v>
+        <v>17</v>
       </c>
       <c r="H51" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="I51">
-        <v>155000</v>
+        <v>200000</v>
       </c>
       <c r="J51" t="s">
-        <v>78</v>
-      </c>
-      <c r="K51">
-        <v>285000000</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>